<commit_message>
Update test order and refactor tests for date inputs
Enhanced end-to-end tests in SaveATrainMixE2EForTrainItaliaTests.java by introducing ordered test execution. Moreover, departure and return dates in MainPage.java are now handled by using LocalDate instead of manually clicking, improving accuracy and efficiency. Upgraded version of dependencies in pom.xml.
</commit_message>
<xml_diff>
--- a/src/test/resources/ConnectionsNSI.xlsx
+++ b/src/test/resources/ConnectionsNSI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalst/IdeaProjects/SaveATrainPlaywrith/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FB2E89-8020-064D-9AFD-25C4AA310E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC656D65-61F7-A54A-B63B-E2D9D6D28709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17400" xr2:uid="{800225BC-0EDC-F14A-9F21-CBE6997CEC23}"/>
   </bookViews>
@@ -34,16 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>SAT_DE_BE_EODMS</t>
-  </si>
-  <si>
-    <t>SAT_IT_MI_PFLRJ</t>
-  </si>
-  <si>
-    <t>SAT_DE_HA_NJFMU</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>SAT_NL_AM_WGRFL</t>
   </si>
@@ -55,9 +46,6 @@
   </si>
   <si>
     <t>SAT_UK_LO_DXLIF</t>
-  </si>
-  <si>
-    <t>SAT_IT_RO_JXWUR</t>
   </si>
   <si>
     <t>originUID</t>
@@ -422,7 +410,7 @@
   <dimension ref="A1:C7572"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,21 +422,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
         <v>45379.292361111111</v>
@@ -456,36 +444,20 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1">
         <v>45379.292361111111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45379.292361111111</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>45379.292361111111</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>

</xml_diff>